<commit_message>
update with clean report
</commit_message>
<xml_diff>
--- a/src/test/resources/test_results.xlsx
+++ b/src/test/resources/test_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="24">
   <si>
     <t>Test Case</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>{"timestamp":"2025-01-02T10:30:46.188+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T11:20:20.322+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
   </si>
 </sst>
 </file>
@@ -125,7 +128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -495,6 +498,76 @@
         <v>22</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
updated with simple loging
</commit_message>
<xml_diff>
--- a/src/test/resources/test_results.xlsx
+++ b/src/test/resources/test_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="31">
   <si>
     <t>Test Case</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>{"timestamp":"2025-01-02T11:20:20.322+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T11:42:05.701+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T11:50:01.626+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T11:59:19.102+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T12:21:42.961+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T12:22:54.587+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T12:26:44.353+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T12:28:15.332+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
   </si>
 </sst>
 </file>
@@ -128,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -568,6 +589,496 @@
         <v>23</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D60" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D65" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D66" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
updated the service to get token directly
</commit_message>
<xml_diff>
--- a/src/test/resources/test_results.xlsx
+++ b/src/test/resources/test_results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="32">
   <si>
     <t>Test Case</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>{"timestamp":"2025-01-02T12:28:15.332+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
+  </si>
+  <si>
+    <t>{"timestamp":"2025-01-02T13:08:17.564+00:00","status":400,"error":"Bad Request","path":"/api/videogame"}</t>
   </si>
 </sst>
 </file>
@@ -149,7 +152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1079,6 +1082,76 @@
         <v>30</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D68" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="B70" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D70" t="s" s="0">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="D71" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>